<commit_message>
Fixses issue on Navbar Higlight tab &  codewords lessthan students
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -1,15 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s530473\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{92F2C0CF-4788-41C5-8C04-E16CE54BDFFF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,28 +20,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
   <si>
-    <t>Testcodeword1</t>
+    <t>S530742@nwmissouri.edu</t>
   </si>
   <si>
-    <t>Testcodeword2</t>
+    <t>Naveen</t>
   </si>
   <si>
-    <t>Testcodeword3</t>
+    <t>bob@bob.com</t>
   </si>
   <si>
-    <t>Testcodeword4</t>
+    <t>Bobby</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -68,13 +72,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -352,39 +359,69 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{A69636EC-9141-431B-A162-76D7F0BCF98A}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{A5608CC4-6539-45DE-B267-A9231AC86E92}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{B3C525BF-565F-467E-8A0F-6B6DFEF58D1A}"/>
+    <hyperlink ref="A4" r:id="rId4" xr:uid="{BA7C9462-A822-4033-84F8-0BE9D7CDFA2F}"/>
+    <hyperlink ref="A5" r:id="rId5" xr:uid="{8F5D6FB0-BE7D-414C-97CF-59430245277D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>